<commit_message>
HRMS sql code addded
</commit_message>
<xml_diff>
--- a/video6HomeworkHRMS/SQL.xlsx
+++ b/video6HomeworkHRMS/SQL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaCamp\video6HomeworkHRMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3EB308B-BB68-463F-8B9D-D2899739CD98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACA810F-A211-4111-9D3A-51E08905735E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>Users</t>
   </si>
@@ -39,36 +39,6 @@
     <t>Employers</t>
   </si>
   <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>identityNumber</t>
-  </si>
-  <si>
-    <t>birthOfYear</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>companyName</t>
-  </si>
-  <si>
-    <t>phoneNumber</t>
-  </si>
-  <si>
-    <t>pssword</t>
-  </si>
-  <si>
-    <t>VerificationCodes</t>
-  </si>
-  <si>
     <t>code</t>
   </si>
   <si>
@@ -78,52 +48,76 @@
     <t>verifiedDate</t>
   </si>
   <si>
-    <t>VerificationCodeCandidates</t>
-  </si>
-  <si>
-    <t>verificationCodeId</t>
-  </si>
-  <si>
-    <t>candidateId</t>
-  </si>
-  <si>
-    <t>VerificationCodeEmloyeers</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
-    <t>userId</t>
-  </si>
-  <si>
-    <t>EmployeeConfirms</t>
-  </si>
-  <si>
-    <t>employeeId</t>
-  </si>
-  <si>
-    <t>isConfirmed</t>
-  </si>
-  <si>
-    <t>confirmDate</t>
-  </si>
-  <si>
-    <t>employeeConfirmId</t>
-  </si>
-  <si>
-    <t>emloyerId</t>
-  </si>
-  <si>
-    <t>employerId</t>
-  </si>
-  <si>
-    <t>webAddress</t>
-  </si>
-  <si>
-    <t>JobTitles</t>
-  </si>
-  <si>
-    <t>titleName</t>
+    <t>identity_number</t>
+  </si>
+  <si>
+    <t>birth_year</t>
+  </si>
+  <si>
+    <t>company_name</t>
+  </si>
+  <si>
+    <t>web_address</t>
+  </si>
+  <si>
+    <t>phone_number</t>
+  </si>
+  <si>
+    <t>verification_codes</t>
+  </si>
+  <si>
+    <t>erification_code_candidates</t>
+  </si>
+  <si>
+    <t>candidate_id</t>
+  </si>
+  <si>
+    <t>Verification_code_emloyeers</t>
+  </si>
+  <si>
+    <t>employer_id</t>
+  </si>
+  <si>
+    <t>employee_id</t>
+  </si>
+  <si>
+    <t>is_confirmed</t>
+  </si>
+  <si>
+    <t>confirm_date</t>
+  </si>
+  <si>
+    <t>employee_confirms</t>
+  </si>
+  <si>
+    <t>employee_confirm_employers</t>
+  </si>
+  <si>
+    <t>job_titels</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>id(int,identity)</t>
+  </si>
+  <si>
+    <t>email(string, unique, not null)</t>
+  </si>
+  <si>
+    <t>password(string, not null)</t>
+  </si>
+  <si>
+    <t>id(int, primary key, foreign key)</t>
+  </si>
+  <si>
+    <t>first_name(string, not null)</t>
+  </si>
+  <si>
+    <t>last_name(string, not null)</t>
   </si>
 </sst>
 </file>
@@ -489,7 +483,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -519,30 +513,30 @@
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
@@ -550,35 +544,29 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E6" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.4">
@@ -586,42 +574,42 @@
         <v>13</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -629,45 +617,45 @@
     </row>
     <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" t="s">
         <v>24</v>
-      </c>
-      <c r="C24" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>